<commit_message>
getting rid of ExcelSKU for speed
</commit_message>
<xml_diff>
--- a/Current Lot Code Data 2.xlsx
+++ b/Current Lot Code Data 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://petreleaf.sharepoint.com/sites/production-warehouse/Shared Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6046" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{108A3D4B-87D5-49B5-9FDD-77891FBF7FEA}"/>
+  <xr:revisionPtr revIDLastSave="6142" documentId="8_{8E997756-1BE6-4E22-AD39-8CBCC25A7D13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{031A64E2-5248-4205-81E5-2FBA5DD3AA37}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
+    <workbookView xWindow="29100" yWindow="1905" windowWidth="14295" windowHeight="15405" xr2:uid="{E068F5DE-AD3F-496A-8413-33EBF2D4DDCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="99">
   <si>
     <t>SKU</t>
   </si>
@@ -84,21 +84,12 @@
     <t>Date</t>
   </si>
   <si>
-    <t>TS-STRESS-PB</t>
-  </si>
-  <si>
-    <t>TS-HJ-PB</t>
-  </si>
-  <si>
     <t>100-DR-HO</t>
   </si>
   <si>
     <t>0524T117</t>
   </si>
   <si>
-    <t>ITCHY &amp; DRY SK-CT</t>
-  </si>
-  <si>
     <t>PRID10042</t>
   </si>
   <si>
@@ -111,15 +102,6 @@
     <t xml:space="preserve">  </t>
   </si>
   <si>
-    <t>HJ-PB-SML</t>
-  </si>
-  <si>
-    <t>SENSITIVE SK-CT</t>
-  </si>
-  <si>
-    <t>STRESS -PB-SML</t>
-  </si>
-  <si>
     <t>200-DR-HO</t>
   </si>
   <si>
@@ -129,36 +111,21 @@
     <t>PRSS0040</t>
   </si>
   <si>
-    <t>HJ-PB-LRG</t>
-  </si>
-  <si>
     <t>500-DR-HO</t>
   </si>
   <si>
-    <t>2 IN 1 SK-CT</t>
-  </si>
-  <si>
     <t>PR2&amp;10041</t>
   </si>
   <si>
     <t>0624T516</t>
   </si>
   <si>
-    <t>STRESS-PB-LRG</t>
-  </si>
-  <si>
-    <t>HJ-PB-FAM</t>
-  </si>
-  <si>
     <t>750-DR-HO</t>
   </si>
   <si>
     <t>0224T409</t>
   </si>
   <si>
-    <t>CONDITIONER SK-CT</t>
-  </si>
-  <si>
     <t>PRC0043</t>
   </si>
   <si>
@@ -183,9 +150,6 @@
     <t>0924FH307</t>
   </si>
   <si>
-    <t>STRESS-PB-FAM</t>
-  </si>
-  <si>
     <t>PRIDS0044</t>
   </si>
   <si>
@@ -198,12 +162,6 @@
     <t>2406P-2</t>
   </si>
   <si>
-    <t>TS-2 IN 1 SHAMPOO</t>
-  </si>
-  <si>
-    <t>TS-STRESS-PEPP</t>
-  </si>
-  <si>
     <t>0924FH609</t>
   </si>
   <si>
@@ -222,12 +180,6 @@
     <t>0822EJ2401</t>
   </si>
   <si>
-    <t>STRESS-PEPP-SML</t>
-  </si>
-  <si>
-    <t>ITCHY-DRY SHAMPOO-GALLON</t>
-  </si>
-  <si>
     <t>PRIDSG0031</t>
   </si>
   <si>
@@ -237,27 +189,18 @@
     <t>2404P</t>
   </si>
   <si>
-    <t>DR - BC - SML</t>
-  </si>
-  <si>
     <t>SK-PW-RL</t>
   </si>
   <si>
     <t>0324CC06</t>
   </si>
   <si>
-    <t>STRESS-PEPP-LRG</t>
-  </si>
-  <si>
     <t>POST-BIO-GH</t>
   </si>
   <si>
     <t>2406X</t>
   </si>
   <si>
-    <t>DR-BC-LRG</t>
-  </si>
-  <si>
     <t>SNT30</t>
   </si>
   <si>
@@ -267,12 +210,6 @@
     <t xml:space="preserve">Yellow Bowl </t>
   </si>
   <si>
-    <t>DR-SP-SML</t>
-  </si>
-  <si>
-    <t>450 Cap</t>
-  </si>
-  <si>
     <t>1123C101</t>
   </si>
   <si>
@@ -285,24 +222,15 @@
     <t>0824FS311</t>
   </si>
   <si>
-    <t>DR-SP-LRG</t>
-  </si>
-  <si>
     <t>600-SR-HO</t>
   </si>
   <si>
     <t>0824FS608</t>
   </si>
   <si>
-    <t>CAT-180</t>
-  </si>
-  <si>
     <t>0624FR1807</t>
   </si>
   <si>
-    <t>150-SR-MINI</t>
-  </si>
-  <si>
     <t>0824FS311-1</t>
   </si>
   <si>
@@ -346,6 +274,90 @@
   </si>
   <si>
     <t>1124U301</t>
+  </si>
+  <si>
+    <t>159360</t>
+  </si>
+  <si>
+    <t>158236</t>
+  </si>
+  <si>
+    <t>158226</t>
+  </si>
+  <si>
+    <t>158225</t>
+  </si>
+  <si>
+    <t>TS-EDI-STRESS-PB</t>
+  </si>
+  <si>
+    <t>EDI-STRESS-PB-LRG</t>
+  </si>
+  <si>
+    <t>EDI-STRESS-PB-FAM</t>
+  </si>
+  <si>
+    <t>TS-EDI-STRESS-PEPP</t>
+  </si>
+  <si>
+    <t>EDI-STRESS-PB-SML</t>
+  </si>
+  <si>
+    <t>EDI-STRESS-PEPP-SML</t>
+  </si>
+  <si>
+    <t>EDI-STRESS-PEPP-LRG</t>
+  </si>
+  <si>
+    <t>TS-EDI-HJ-PB</t>
+  </si>
+  <si>
+    <t>EDI-HJ-PB-SML</t>
+  </si>
+  <si>
+    <t>EDI-HJ-PB-LRG</t>
+  </si>
+  <si>
+    <t>EDI-HJ-PB-FAM</t>
+  </si>
+  <si>
+    <t>EDI-DR-BC-SML</t>
+  </si>
+  <si>
+    <t>EDI-DR-BC-LRG</t>
+  </si>
+  <si>
+    <t>EDI-DR-SP-SML</t>
+  </si>
+  <si>
+    <t>EDI-DR-SP-LRG</t>
+  </si>
+  <si>
+    <t>ITCHY &amp; DRY-SK-CT</t>
+  </si>
+  <si>
+    <t>SENSITIVE-SK-CT</t>
+  </si>
+  <si>
+    <t>CONDITIONER-SK-CT</t>
+  </si>
+  <si>
+    <t>2IN1-SK-CT</t>
+  </si>
+  <si>
+    <t>TS-2IN1-SHAMPOO</t>
+  </si>
+  <si>
+    <t>ITCHY-DRY-SHAMPOO-GALLON</t>
+  </si>
+  <si>
+    <t>Cap450</t>
+  </si>
+  <si>
+    <t>180-CAT-SR</t>
+  </si>
+  <si>
+    <t>150-MINI-STRESS-HO</t>
   </si>
 </sst>
 </file>
@@ -695,6 +707,16 @@
     <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -705,16 +727,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1059,14 +1071,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4D02CE-C7F3-446F-985C-950AF7BFACB9}">
   <dimension ref="A1:AE283"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
     <col min="3" max="3" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" style="4" customWidth="1"/>
@@ -1183,26 +1195,26 @@
     </row>
     <row r="2" spans="1:31" ht="27.95" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="23" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="G2" s="32"/>
       <c r="H2" s="23" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="N2" s="32"/>
       <c r="O2" s="23" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="U2" s="32"/>
       <c r="V2" s="43" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="AB2" s="8"/>
       <c r="AE2" s="18"/>
     </row>
     <row r="3" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
-        <v>7</v>
+        <v>75</v>
       </c>
       <c r="B3" s="7">
         <v>158584</v>
@@ -1217,12 +1229,12 @@
         <v>46251</v>
       </c>
       <c r="F3" s="9">
-        <f t="shared" ref="F3:F4" si="0">(E3-$AC$1)/365*12</f>
+        <f t="shared" ref="F3:F5" si="0">(E3-$AC$1)/365*12</f>
         <v>20.843835616438355</v>
       </c>
       <c r="G3" s="33"/>
       <c r="H3" s="6" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="I3" s="7">
         <v>155511</v>
@@ -1242,10 +1254,10 @@
       </c>
       <c r="N3" s="33"/>
       <c r="O3" s="6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="P3" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q3" s="12">
         <v>3</v>
@@ -1262,10 +1274,10 @@
       </c>
       <c r="U3" s="33"/>
       <c r="V3" s="6" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="W3" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="X3" s="7">
         <v>0</v>
@@ -1317,7 +1329,7 @@
       <c r="N4" s="33"/>
       <c r="O4" s="27"/>
       <c r="P4" s="7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="Q4" s="7">
         <v>7</v>
@@ -1332,7 +1344,7 @@
       </c>
       <c r="U4" s="33"/>
       <c r="W4" s="7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="X4" s="15">
         <v>102</v>
@@ -1348,15 +1360,20 @@
       <c r="AB4" s="7"/>
     </row>
     <row r="5" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="44">
-        <f>SUM(C3:C4)*40+D3</f>
-        <v>6199</v>
-      </c>
-      <c r="D5" s="45"/>
-      <c r="F5" s="7"/>
+      <c r="B5" s="41">
+        <v>163236</v>
+      </c>
+      <c r="C5" s="41">
+        <v>100</v>
+      </c>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42">
+        <v>46323</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="0"/>
+        <v>23.210958904109589</v>
+      </c>
       <c r="G5" s="33"/>
       <c r="I5" s="7">
         <v>158587</v>
@@ -1375,7 +1392,7 @@
       <c r="N5" s="33"/>
       <c r="O5" s="27"/>
       <c r="P5" s="7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Q5" s="7">
         <v>202</v>
@@ -1392,71 +1409,61 @@
       </c>
       <c r="U5" s="33"/>
       <c r="W5" s="7"/>
-      <c r="X5" s="44">
+      <c r="X5" s="48">
         <f>SUM(X3:X4)*6+Y3+Y4</f>
         <v>617</v>
       </c>
-      <c r="Y5" s="45"/>
+      <c r="Y5" s="49"/>
       <c r="AB5" s="7"/>
     </row>
     <row r="6" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="48">
+        <f>SUM(C3:C5)*40+D3</f>
+        <v>10199</v>
+      </c>
+      <c r="D6" s="49"/>
       <c r="F6" s="7"/>
       <c r="G6" s="33"/>
       <c r="I6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="44">
+        <v>10</v>
+      </c>
+      <c r="J6" s="48">
         <f>SUM(J3:J5)*40+K3</f>
         <v>6373</v>
       </c>
-      <c r="K6" s="45"/>
+      <c r="K6" s="49"/>
       <c r="N6" s="33"/>
       <c r="P6" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q6" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q6" s="48">
         <f>SUM(Q3:Q5)*30+R3+R5</f>
         <v>6379</v>
       </c>
-      <c r="R6" s="45"/>
+      <c r="R6" s="49"/>
       <c r="U6" s="33"/>
       <c r="V6" s="10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="AB6" s="7"/>
     </row>
     <row r="7" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="7">
-        <v>156639</v>
-      </c>
-      <c r="C7" s="7">
-        <v>2</v>
-      </c>
-      <c r="D7" s="7">
-        <v>19</v>
-      </c>
-      <c r="E7" s="8">
-        <v>46157</v>
-      </c>
-      <c r="F7" s="9">
-        <f t="shared" ref="F7" si="7">(E7-$AC$1)/365*12</f>
-        <v>17.753424657534246</v>
-      </c>
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="33"/>
       <c r="K7" s="7"/>
       <c r="N7" s="33"/>
       <c r="U7" s="33"/>
       <c r="V7" s="6" t="s">
-        <v>17</v>
+        <v>91</v>
       </c>
       <c r="W7" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="X7" s="15">
         <v>0</v>
@@ -1468,30 +1475,34 @@
         <v>46993</v>
       </c>
       <c r="AA7" s="9">
-        <f t="shared" ref="AA7" si="8">(Z7-$AC$1)/365*12</f>
+        <f t="shared" ref="AA7" si="7">(Z7-$AC$1)/365*12</f>
         <v>45.238356164383561</v>
       </c>
       <c r="AB7" s="7"/>
     </row>
     <row r="8" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="27"/>
+      <c r="A8" s="6" t="s">
+        <v>79</v>
+      </c>
       <c r="B8" s="7">
         <v>156639</v>
       </c>
-      <c r="C8" s="11">
-        <v>43</v>
-      </c>
-      <c r="D8" s="7"/>
+      <c r="C8" s="7">
+        <v>2</v>
+      </c>
+      <c r="D8" s="7">
+        <v>19</v>
+      </c>
       <c r="E8" s="8">
         <v>46157</v>
       </c>
       <c r="F8" s="9">
-        <f>(E8-$AC$1)/365*12</f>
+        <f t="shared" ref="F8" si="8">(E8-$AC$1)/365*12</f>
         <v>17.753424657534246</v>
       </c>
       <c r="G8" s="33"/>
       <c r="H8" s="6" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="I8" s="7">
         <v>156645</v>
@@ -1511,10 +1522,10 @@
       </c>
       <c r="N8" s="33"/>
       <c r="O8" s="6" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="P8" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="Q8" s="7">
         <v>7</v>
@@ -1531,7 +1542,7 @@
       </c>
       <c r="U8" s="33"/>
       <c r="W8" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="X8" s="7">
         <v>62</v>
@@ -1551,18 +1562,18 @@
     <row r="9" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="27"/>
       <c r="B9" s="7">
-        <v>158223</v>
+        <v>156639</v>
       </c>
       <c r="C9" s="11">
-        <v>161</v>
+        <v>43</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="8">
-        <v>46185</v>
+        <v>46157</v>
       </c>
       <c r="F9" s="9">
         <f>(E9-$AC$1)/365*12</f>
-        <v>18.673972602739727</v>
+        <v>17.753424657534246</v>
       </c>
       <c r="G9" s="33"/>
       <c r="H9" s="27"/>
@@ -1584,7 +1595,7 @@
       </c>
       <c r="N9" s="33"/>
       <c r="P9" s="7" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="Q9" s="7">
         <v>160</v>
@@ -1601,71 +1612,77 @@
       </c>
       <c r="U9" s="33"/>
       <c r="W9" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X9" s="44">
+        <v>10</v>
+      </c>
+      <c r="X9" s="48">
         <f>SUM(X7:X8)*6+Y7</f>
         <v>377</v>
       </c>
-      <c r="Y9" s="45"/>
+      <c r="Y9" s="49"/>
       <c r="AB9" s="7"/>
     </row>
     <row r="10" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="27"/>
       <c r="B10" s="7">
-        <v>158583</v>
+        <v>158223</v>
       </c>
       <c r="C10" s="11">
-        <v>81</v>
+        <v>161</v>
       </c>
       <c r="D10" s="7"/>
       <c r="E10" s="8">
-        <v>46250</v>
+        <v>46185</v>
       </c>
       <c r="F10" s="9">
         <f>(E10-$AC$1)/365*12</f>
-        <v>20.81095890410959</v>
+        <v>18.673972602739727</v>
       </c>
       <c r="G10" s="33"/>
       <c r="I10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="44">
+        <v>10</v>
+      </c>
+      <c r="J10" s="48">
         <f>SUM(J8:J9)*24+K8</f>
         <v>4841</v>
       </c>
-      <c r="K10" s="45"/>
+      <c r="K10" s="49"/>
       <c r="N10" s="33"/>
       <c r="P10" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q10" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q10" s="48">
         <f>SUM(Q8:Q9)*30+R8+R9</f>
         <v>5043</v>
       </c>
-      <c r="R10" s="45"/>
+      <c r="R10" s="49"/>
       <c r="U10" s="33"/>
       <c r="AB10" s="7"/>
     </row>
     <row r="11" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C11" s="44">
-        <f>SUM(C7:C10)*24+D7</f>
-        <v>6907</v>
-      </c>
-      <c r="D11" s="45"/>
-      <c r="F11" s="7"/>
+      <c r="A11" s="27"/>
+      <c r="B11" s="7">
+        <v>158583</v>
+      </c>
+      <c r="C11" s="11">
+        <v>164</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8">
+        <v>46250</v>
+      </c>
+      <c r="F11" s="9">
+        <f>(E11-$AC$1)/365*12</f>
+        <v>20.81095890410959</v>
+      </c>
       <c r="G11" s="33"/>
       <c r="K11" s="7"/>
       <c r="N11" s="33"/>
       <c r="U11" s="33"/>
       <c r="V11" s="6" t="s">
-        <v>24</v>
+        <v>93</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="X11" s="7">
         <v>3</v>
@@ -1683,11 +1700,18 @@
       <c r="AB11" s="7"/>
     </row>
     <row r="12" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="7"/>
+      <c r="B12" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="48">
+        <f>SUM(C8:C11)*24+D8</f>
+        <v>8899</v>
+      </c>
+      <c r="D12" s="49"/>
       <c r="F12" s="7"/>
       <c r="G12" s="33"/>
       <c r="H12" s="6" t="s">
-        <v>22</v>
+        <v>84</v>
       </c>
       <c r="I12" s="7">
         <v>158212</v>
@@ -1707,10 +1731,10 @@
       </c>
       <c r="N12" s="33"/>
       <c r="O12" s="6" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P12" s="7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="Q12" s="7">
         <v>3</v>
@@ -1727,7 +1751,7 @@
       </c>
       <c r="U12" s="33"/>
       <c r="W12" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="X12" s="7">
         <v>55</v>
@@ -1743,21 +1767,8 @@
       <c r="AB12" s="7"/>
     </row>
     <row r="13" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="35">
-        <v>158219</v>
-      </c>
-      <c r="C13" s="7">
-        <v>6</v>
-      </c>
-      <c r="D13" s="7">
-        <v>22</v>
-      </c>
-      <c r="E13" s="8">
-        <v>46191</v>
-      </c>
+      <c r="D13" s="7"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="33"/>
       <c r="H13" s="27"/>
       <c r="I13" s="7">
@@ -1777,7 +1788,7 @@
       <c r="N13" s="33"/>
       <c r="O13" s="27"/>
       <c r="P13" s="7" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="Q13" s="7">
         <v>88</v>
@@ -1794,29 +1805,34 @@
       </c>
       <c r="U13" s="33"/>
       <c r="W13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X13" s="44">
+        <v>10</v>
+      </c>
+      <c r="X13" s="48">
         <f>SUM(X11:X12)*6+Y11+Y12</f>
         <v>351</v>
       </c>
-      <c r="Y13" s="45"/>
+      <c r="Y13" s="49"/>
       <c r="AB13" s="7"/>
     </row>
     <row r="14" spans="1:31" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="6" t="s">
+        <v>76</v>
+      </c>
       <c r="B14" s="35">
-        <v>158219</v>
-      </c>
-      <c r="C14" s="11">
-        <v>12</v>
-      </c>
-      <c r="D14" s="7"/>
+        <v>158220</v>
+      </c>
+      <c r="C14" s="7">
+        <v>6</v>
+      </c>
+      <c r="D14" s="7">
+        <v>6</v>
+      </c>
       <c r="E14" s="8">
-        <v>46191</v>
+        <v>46197</v>
       </c>
       <c r="F14" s="9">
         <f>(E14-$AC$1)/365*12</f>
-        <v>18.871232876712327</v>
+        <v>19.06849315068493</v>
       </c>
       <c r="G14" s="33"/>
       <c r="H14" s="27"/>
@@ -1836,13 +1852,13 @@
       </c>
       <c r="N14" s="33"/>
       <c r="P14" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q14" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="48">
         <f>SUM(Q12:Q13)*30+R12</f>
         <v>2756</v>
       </c>
-      <c r="R14" s="45"/>
+      <c r="R14" s="49"/>
       <c r="U14" s="33"/>
       <c r="AB14" s="7"/>
     </row>
@@ -1851,7 +1867,7 @@
         <v>158220</v>
       </c>
       <c r="C15" s="11">
-        <v>159</v>
+        <v>21</v>
       </c>
       <c r="D15" s="7"/>
       <c r="E15" s="8">
@@ -1862,21 +1878,28 @@
         <v>19.06849315068493</v>
       </c>
       <c r="G15" s="33"/>
-      <c r="I15" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J15" s="44">
-        <f>SUM(J12:J14)*24+K12</f>
-        <v>5031</v>
-      </c>
-      <c r="K15" s="45"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="7">
+        <v>163239</v>
+      </c>
+      <c r="J15" s="7">
+        <v>171</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="8">
+        <v>46311</v>
+      </c>
+      <c r="M15" s="9">
+        <f>(L15-$AC$1)/365*12</f>
+        <v>22.816438356164383</v>
+      </c>
       <c r="N15" s="33"/>
       <c r="U15" s="33"/>
       <c r="V15" s="6" t="s">
-        <v>31</v>
+        <v>92</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="X15" s="7">
         <v>4</v>
@@ -1898,7 +1921,7 @@
         <v>158221</v>
       </c>
       <c r="C16" s="11">
-        <v>160</v>
+        <v>335</v>
       </c>
       <c r="D16" s="7"/>
       <c r="E16" s="8">
@@ -1909,13 +1932,20 @@
         <v>20.778082191780822</v>
       </c>
       <c r="G16" s="33"/>
-      <c r="K16" s="7"/>
+      <c r="I16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="48">
+        <f>SUM(J12:J15)*24+K12</f>
+        <v>9135</v>
+      </c>
+      <c r="K16" s="49"/>
       <c r="N16" s="33"/>
       <c r="O16" s="6" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="P16" s="7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="Q16" s="7">
         <v>3</v>
@@ -1933,7 +1963,7 @@
       <c r="U16" s="33"/>
       <c r="V16" s="6"/>
       <c r="W16" s="7" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="X16" s="7">
         <v>47</v>
@@ -1952,37 +1982,19 @@
     </row>
     <row r="17" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="44">
-        <f>SUM(C14:C15)*24+D14</f>
-        <v>4104</v>
-      </c>
-      <c r="D17" s="45"/>
+        <v>10</v>
+      </c>
+      <c r="C17" s="48">
+        <f>SUM(C14:C16)*24+D14</f>
+        <v>8694</v>
+      </c>
+      <c r="D17" s="49"/>
       <c r="F17" s="7"/>
       <c r="G17" s="33"/>
-      <c r="H17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="I17" s="7">
-        <v>156646</v>
-      </c>
-      <c r="J17" s="7">
-        <v>4</v>
-      </c>
-      <c r="K17" s="11">
-        <v>6</v>
-      </c>
-      <c r="L17" s="8">
-        <v>46192</v>
-      </c>
-      <c r="M17" s="9">
-        <f t="shared" ref="M17" si="19">(L17-$AC$1)/365*12</f>
-        <v>18.904109589041099</v>
-      </c>
+      <c r="K17" s="7"/>
       <c r="N17" s="33"/>
       <c r="P17" s="7" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="Q17" s="7">
         <v>21</v>
@@ -1994,92 +2006,103 @@
         <v>46199</v>
       </c>
       <c r="T17" s="9">
-        <f t="shared" ref="T17" si="20">(S17-$AC$1)/365*12</f>
+        <f t="shared" ref="T17" si="19">(S17-$AC$1)/365*12</f>
         <v>19.134246575342466</v>
       </c>
       <c r="U17" s="33"/>
       <c r="W17" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X17" s="44">
+        <v>10</v>
+      </c>
+      <c r="X17" s="48">
         <f>SUM(X15:X16)*6+Y15+Y16</f>
         <v>310</v>
       </c>
-      <c r="Y17" s="45"/>
+      <c r="Y17" s="49"/>
       <c r="AB17" s="7"/>
     </row>
     <row r="18" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="48"/>
+      <c r="B18" s="44"/>
       <c r="D18" s="7"/>
       <c r="F18" s="7"/>
       <c r="G18" s="33"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="6" t="s">
+        <v>85</v>
+      </c>
       <c r="I18" s="7">
         <v>156646</v>
       </c>
       <c r="J18" s="7">
-        <v>163</v>
-      </c>
-      <c r="K18" s="11"/>
+        <v>4</v>
+      </c>
+      <c r="K18" s="11">
+        <v>6</v>
+      </c>
       <c r="L18" s="8">
         <v>46192</v>
       </c>
       <c r="M18" s="9">
-        <f t="shared" ref="M18" si="21">(L18-$AC$1)/365*12</f>
+        <f t="shared" ref="M18" si="20">(L18-$AC$1)/365*12</f>
         <v>18.904109589041099</v>
       </c>
       <c r="N18" s="33"/>
       <c r="P18" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q18" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="48">
         <f>SUM(Q16:Q17)*30+R16+R17</f>
         <v>754</v>
       </c>
-      <c r="R18" s="45"/>
+      <c r="R18" s="49"/>
       <c r="U18" s="33"/>
       <c r="AB18" s="7"/>
     </row>
-    <row r="19" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B19" s="49">
+        <v>77</v>
+      </c>
+      <c r="B19" s="45">
         <v>158225</v>
       </c>
       <c r="C19" s="7">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D19" s="7">
-        <v>8</v>
-      </c>
-      <c r="E19" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="E19" s="8">
+        <v>46191</v>
+      </c>
       <c r="F19" s="9">
         <f>(E19-$AC$1)/365*12</f>
-        <v>-1499.7369863013701</v>
+        <v>18.871232876712327</v>
       </c>
       <c r="G19" s="33"/>
-      <c r="I19" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J19" s="44">
-        <f>SUM(J17:J18)*12+K17</f>
-        <v>2010</v>
-      </c>
-      <c r="K19" s="45"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="7"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7">
+        <v>156646</v>
+      </c>
+      <c r="J19" s="7">
+        <v>163</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="8">
+        <v>46192</v>
+      </c>
+      <c r="M19" s="9">
+        <f t="shared" ref="M19:M20" si="21">(L19-$AC$1)/365*12</f>
+        <v>18.904109589041099</v>
+      </c>
       <c r="N19" s="33"/>
       <c r="P19" s="13"/>
       <c r="Q19" s="10" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="U19" s="33"/>
       <c r="V19" s="6" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="X19" s="7">
         <v>0</v>
@@ -2097,26 +2120,43 @@
       <c r="AB19" s="7"/>
     </row>
     <row r="20" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="27"/>
-      <c r="B20" s="49">
-        <v>158225</v>
+      <c r="A20" s="6"/>
+      <c r="B20" s="45" t="s">
+        <v>74</v>
       </c>
       <c r="C20" s="7">
-        <v>53</v>
-      </c>
-      <c r="E20" s="8"/>
+        <v>47</v>
+      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="8">
+        <v>46191</v>
+      </c>
       <c r="F20" s="9">
         <f>(E20-$AC$1)/365*12</f>
-        <v>-1499.7369863013701</v>
+        <v>18.871232876712327</v>
       </c>
       <c r="G20" s="33"/>
-      <c r="K20" s="7"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7">
+        <v>163238</v>
+      </c>
+      <c r="J20" s="7">
+        <v>104</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="8">
+        <v>46310</v>
+      </c>
+      <c r="M20" s="9">
+        <f t="shared" si="21"/>
+        <v>22.783561643835618</v>
+      </c>
       <c r="N20" s="33"/>
       <c r="O20" s="6" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="P20" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="Q20" s="7">
         <v>4</v>
@@ -2136,7 +2176,7 @@
         <v>200</v>
       </c>
       <c r="W20" s="7" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="X20" s="7">
         <v>7</v>
@@ -2155,7 +2195,7 @@
     </row>
     <row r="21" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="27"/>
-      <c r="B21" s="49">
+      <c r="B21" s="45">
         <v>156626</v>
       </c>
       <c r="C21" s="7">
@@ -2169,28 +2209,19 @@
         <v>18.871232876712327</v>
       </c>
       <c r="G21" s="33"/>
-      <c r="H21" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J21" s="7">
-        <v>5</v>
-      </c>
-      <c r="K21" s="7">
-        <v>5</v>
-      </c>
-      <c r="L21" s="14">
-        <v>46291</v>
-      </c>
-      <c r="M21" s="9">
-        <f t="shared" ref="M21" si="25">(L21-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
-      </c>
+      <c r="I21" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="48">
+        <f>SUM(J18:J20)*12+K18</f>
+        <v>3258</v>
+      </c>
+      <c r="K21" s="49"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="33"/>
       <c r="P21" s="7" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="Q21" s="7">
         <v>92</v>
@@ -2207,68 +2238,77 @@
       </c>
       <c r="U21" s="33"/>
       <c r="W21" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X21" s="44">
+        <v>10</v>
+      </c>
+      <c r="X21" s="48">
         <v>1973</v>
       </c>
-      <c r="Y21" s="45"/>
+      <c r="Y21" s="49"/>
       <c r="AB21" s="7"/>
     </row>
     <row r="22" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C22" s="44">
-        <f>SUM(C19:C21)*12+D19</f>
-        <v>740</v>
-      </c>
-      <c r="D22" s="45"/>
-      <c r="F22" s="7"/>
+      <c r="A22" s="27"/>
+      <c r="B22" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C22" s="7">
+        <v>104</v>
+      </c>
+      <c r="E22" s="8">
+        <v>46198</v>
+      </c>
+      <c r="F22" s="9">
+        <f t="shared" ref="F22" si="25">(E22-$AC$1)/365*12</f>
+        <v>19.101369863013698</v>
+      </c>
       <c r="G22" s="33"/>
-      <c r="I22" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="J22" s="7">
-        <v>49</v>
-      </c>
       <c r="K22" s="7"/>
-      <c r="L22" s="14">
-        <v>46291</v>
-      </c>
-      <c r="M22" s="9">
-        <f t="shared" ref="M22" si="26">(L22-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
-      </c>
       <c r="N22" s="33"/>
       <c r="P22" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q22" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="48">
         <f>SUM(Q20:Q21)*30+R20+R21</f>
         <v>2915</v>
       </c>
-      <c r="R22" s="45"/>
+      <c r="R22" s="49"/>
       <c r="U22" s="33"/>
       <c r="AB22" s="7"/>
     </row>
     <row r="23" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="48"/>
-      <c r="D23" s="7"/>
+      <c r="B23" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="48">
+        <f>SUM(C19:C22)*12+D19</f>
+        <v>1993</v>
+      </c>
+      <c r="D23" s="49"/>
       <c r="F23" s="7"/>
       <c r="G23" s="33"/>
-      <c r="I23" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J23" s="44">
-        <f>SUM(J21:J22)*30+K21+K22</f>
-        <v>1625</v>
-      </c>
-      <c r="K23" s="45"/>
+      <c r="H23" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="7">
+        <v>5</v>
+      </c>
+      <c r="K23" s="7">
+        <v>5</v>
+      </c>
+      <c r="L23" s="14">
+        <v>46291</v>
+      </c>
+      <c r="M23" s="9">
+        <f t="shared" ref="M23" si="26">(L23-$AC$1)/365*12</f>
+        <v>22.158904109589042</v>
+      </c>
       <c r="N23" s="33"/>
       <c r="U23" s="33"/>
       <c r="V23" s="21" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="W23" s="7"/>
       <c r="X23" s="7"/>
@@ -2278,36 +2318,30 @@
       <c r="AB23" s="7"/>
     </row>
     <row r="24" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B24" s="51">
-        <v>158238</v>
-      </c>
-      <c r="C24" s="7">
-        <v>0</v>
-      </c>
-      <c r="D24" s="7">
-        <v>37</v>
-      </c>
-      <c r="E24" s="8">
-        <v>46190</v>
-      </c>
-      <c r="F24" s="9">
-        <f>(E24-$AC$1)/365*12</f>
-        <v>18.838356164383562</v>
-      </c>
+      <c r="B24" s="44"/>
+      <c r="D24" s="7"/>
+      <c r="F24" s="7"/>
       <c r="G24" s="33"/>
+      <c r="I24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="7">
+        <v>49</v>
+      </c>
       <c r="K24" s="7"/>
-      <c r="M24" s="10" t="s">
-        <v>33</v>
+      <c r="L24" s="14">
+        <v>46291</v>
+      </c>
+      <c r="M24" s="9">
+        <f t="shared" ref="M24" si="27">(L24-$AC$1)/365*12</f>
+        <v>22.158904109589042</v>
       </c>
       <c r="N24" s="33"/>
       <c r="O24" s="6" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="P24" s="7" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="Q24" s="7">
         <v>6</v>
@@ -2319,7 +2353,7 @@
         <v>46199</v>
       </c>
       <c r="T24" s="9">
-        <f t="shared" ref="T24:T26" si="27">(S24-$AC$1)/365*12</f>
+        <f t="shared" ref="T24:T26" si="28">(S24-$AC$1)/365*12</f>
         <v>19.134246575342466</v>
       </c>
       <c r="U24" s="33"/>
@@ -2327,7 +2361,7 @@
         <v>200</v>
       </c>
       <c r="W24" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="X24" s="7">
         <v>5</v>
@@ -2339,20 +2373,24 @@
         <v>46993</v>
       </c>
       <c r="AA24" s="9">
-        <f t="shared" ref="AA24" si="28">(Z24-$AC$1)/365*12</f>
+        <f t="shared" ref="AA24" si="29">(Z24-$AC$1)/365*12</f>
         <v>45.238356164383561</v>
       </c>
       <c r="AB24" s="7"/>
     </row>
     <row r="25" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
-      <c r="B25" s="51">
+      <c r="A25" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="47">
         <v>158238</v>
       </c>
-      <c r="C25" s="11">
-        <v>47</v>
-      </c>
-      <c r="D25" s="7"/>
+      <c r="C25" s="7">
+        <v>0</v>
+      </c>
+      <c r="D25" s="7">
+        <v>37</v>
+      </c>
       <c r="E25" s="8">
         <v>46190</v>
       </c>
@@ -2361,28 +2399,17 @@
         <v>18.838356164383562</v>
       </c>
       <c r="G25" s="33"/>
-      <c r="H25" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J25" s="7">
-        <v>5</v>
-      </c>
-      <c r="K25" s="7">
-        <v>26</v>
-      </c>
-      <c r="L25" s="25">
-        <v>46291</v>
-      </c>
-      <c r="M25" s="9">
-        <f t="shared" ref="M25" si="29">(L25-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
-      </c>
+      <c r="I25" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="48">
+        <f>SUM(J23:J24)*30+K23+K24</f>
+        <v>1625</v>
+      </c>
+      <c r="K25" s="49"/>
       <c r="N25" s="33"/>
       <c r="P25" s="7" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="Q25" s="7">
         <v>52</v>
@@ -2394,55 +2421,43 @@
         <v>46199</v>
       </c>
       <c r="T25" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>19.134246575342466</v>
       </c>
       <c r="U25" s="33"/>
       <c r="W25" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X25" s="44">
+        <v>10</v>
+      </c>
+      <c r="X25" s="48">
         <v>1990</v>
       </c>
-      <c r="Y25" s="45"/>
+      <c r="Y25" s="49"/>
       <c r="AB25" s="7"/>
     </row>
     <row r="26" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="29"/>
-      <c r="B26" s="51">
-        <v>163030</v>
+      <c r="B26" s="47">
+        <v>158238</v>
       </c>
       <c r="C26" s="11">
-        <v>100</v>
+        <v>47</v>
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="8">
-        <v>46302</v>
+        <v>46190</v>
       </c>
       <c r="F26" s="9">
         <f>(E26-$AC$1)/365*12</f>
-        <v>22.520547945205479</v>
+        <v>18.838356164383562</v>
       </c>
       <c r="G26" s="33"/>
-      <c r="I26" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="J26" s="7">
-        <v>59</v>
-      </c>
-      <c r="K26" s="7">
-        <v>0</v>
-      </c>
-      <c r="L26" s="25">
-        <v>46291</v>
-      </c>
-      <c r="M26" s="9">
-        <f t="shared" ref="M26" si="30">(L26-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
+      <c r="K26" s="7"/>
+      <c r="M26" s="10" t="s">
+        <v>22</v>
       </c>
       <c r="N26" s="33"/>
       <c r="P26" s="7" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="Q26" s="7">
         <v>50</v>
@@ -2454,49 +2469,66 @@
         <v>46352</v>
       </c>
       <c r="T26" s="9">
-        <f t="shared" si="27"/>
+        <f t="shared" si="28"/>
         <v>24.164383561643838</v>
       </c>
       <c r="U26" s="33"/>
       <c r="AB26" s="7"/>
     </row>
     <row r="27" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B27" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="44">
-        <f>SUM(C25:C25)*40+D25</f>
-        <v>1880</v>
-      </c>
-      <c r="D27" s="45"/>
-      <c r="F27" s="7"/>
+      <c r="A27" s="29"/>
+      <c r="B27" s="47">
+        <v>163030</v>
+      </c>
+      <c r="C27" s="11">
+        <v>100</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="8">
+        <v>46302</v>
+      </c>
+      <c r="F27" s="9">
+        <f>(E27-$AC$1)/365*12</f>
+        <v>22.520547945205479</v>
+      </c>
       <c r="G27" s="33"/>
-      <c r="I27" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J27" s="44">
-        <f>SUM(J25:J26)*30+K25</f>
-        <v>1946</v>
-      </c>
-      <c r="K27" s="45"/>
+      <c r="H27" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="7">
+        <v>5</v>
+      </c>
+      <c r="K27" s="7">
+        <v>26</v>
+      </c>
+      <c r="L27" s="25">
+        <v>46291</v>
+      </c>
+      <c r="M27" s="9">
+        <f t="shared" ref="M27" si="30">(L27-$AC$1)/365*12</f>
+        <v>22.158904109589042</v>
+      </c>
       <c r="N27" s="33"/>
       <c r="P27" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q27" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q27" s="48">
         <f>SUM(Q24:Q26)*30+R24+R25+R26</f>
         <v>3288</v>
       </c>
-      <c r="R27" s="45"/>
+      <c r="R27" s="49"/>
       <c r="U27" s="33"/>
-      <c r="V27" s="46" t="s">
-        <v>54</v>
+      <c r="V27" s="50" t="s">
+        <v>95</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>55</v>
+        <v>39</v>
       </c>
       <c r="X27" s="7">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y27" s="7">
         <v>1</v>
@@ -2511,70 +2543,64 @@
       <c r="AB27" s="7"/>
     </row>
     <row r="28" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="48"/>
-      <c r="D28" s="7"/>
+      <c r="B28" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="48">
+        <f>SUM(C26:C26)*40+D26</f>
+        <v>1880</v>
+      </c>
+      <c r="D28" s="49"/>
       <c r="F28" s="7"/>
       <c r="G28" s="33"/>
-      <c r="K28" s="7"/>
+      <c r="I28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="J28" s="7">
+        <v>59</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0</v>
+      </c>
+      <c r="L28" s="25">
+        <v>46291</v>
+      </c>
+      <c r="M28" s="9">
+        <f t="shared" ref="M28" si="32">(L28-$AC$1)/365*12</f>
+        <v>22.158904109589042</v>
+      </c>
       <c r="N28" s="33"/>
       <c r="U28" s="33"/>
-      <c r="V28" s="46"/>
+      <c r="V28" s="50"/>
       <c r="W28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X28" s="44">
+        <v>10</v>
+      </c>
+      <c r="X28" s="48">
         <f>SUM(X27)*4+Y27</f>
-        <v>9</v>
-      </c>
-      <c r="Y28" s="45"/>
+        <v>1</v>
+      </c>
+      <c r="Y28" s="49"/>
       <c r="AB28" s="7"/>
     </row>
     <row r="29" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B29" s="49">
-        <v>156636</v>
-      </c>
-      <c r="C29" s="7">
-        <v>0</v>
-      </c>
-      <c r="D29" s="7">
-        <v>12</v>
-      </c>
-      <c r="E29" s="8">
-        <v>46156</v>
-      </c>
-      <c r="F29" s="9">
-        <f>(E29-$AC$1)/365*12</f>
-        <v>17.720547945205482</v>
-      </c>
+      <c r="B29" s="44"/>
+      <c r="D29" s="7"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="33"/>
-      <c r="H29" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="J29" s="7">
-        <v>8</v>
-      </c>
-      <c r="K29" s="7">
-        <v>2</v>
-      </c>
-      <c r="L29" s="14">
-        <v>45528</v>
-      </c>
-      <c r="M29" s="16">
-        <f t="shared" ref="M29" si="32">(L29-$AC$1)/365*12</f>
-        <v>-2.9260273972602739</v>
-      </c>
+      <c r="I29" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="48">
+        <f>SUM(J27:J28)*30+K27</f>
+        <v>1946</v>
+      </c>
+      <c r="K29" s="49"/>
       <c r="N29" s="33"/>
       <c r="O29" s="6" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="P29" s="7" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="Q29" s="7">
         <v>3</v>
@@ -2593,13 +2619,18 @@
       <c r="AB29" s="8"/>
     </row>
     <row r="30" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="49">
+      <c r="A30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B30" s="45">
         <v>156636</v>
       </c>
       <c r="C30" s="7">
-        <v>59</v>
-      </c>
-      <c r="D30" s="7"/>
+        <v>0</v>
+      </c>
+      <c r="D30" s="7">
+        <v>12</v>
+      </c>
       <c r="E30" s="8">
         <v>46156</v>
       </c>
@@ -2608,18 +2639,11 @@
         <v>17.720547945205482</v>
       </c>
       <c r="G30" s="33"/>
-      <c r="I30" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J30" s="44">
-        <f>SUM(J29)*30+K29</f>
-        <v>242</v>
-      </c>
-      <c r="K30" s="45"/>
+      <c r="K30" s="7"/>
       <c r="N30" s="33"/>
       <c r="O30" s="6"/>
       <c r="P30" s="7" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="Q30" s="7">
         <v>26</v>
@@ -2634,10 +2658,10 @@
       </c>
       <c r="U30" s="33"/>
       <c r="V30" s="6" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="W30" s="7" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="X30" s="7">
         <v>4</v>
@@ -2654,101 +2678,111 @@
       </c>
     </row>
     <row r="31" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="49">
-        <v>158234</v>
+      <c r="B31" s="45">
+        <v>156636</v>
       </c>
       <c r="C31" s="7">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="8">
-        <v>46191</v>
+        <v>46156</v>
       </c>
       <c r="F31" s="9">
         <f>(E31-$AC$1)/365*12</f>
-        <v>18.871232876712327</v>
+        <v>17.720547945205482</v>
       </c>
       <c r="G31" s="33"/>
-      <c r="K31" s="7"/>
+      <c r="H31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="J31" s="7">
+        <v>8</v>
+      </c>
+      <c r="K31" s="7">
+        <v>2</v>
+      </c>
+      <c r="L31" s="14">
+        <v>45528</v>
+      </c>
+      <c r="M31" s="16">
+        <f t="shared" ref="M31" si="35">(L31-$AC$1)/365*12</f>
+        <v>-2.9260273972602739</v>
+      </c>
       <c r="N31" s="33"/>
       <c r="P31" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q31" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q31" s="48">
         <f>SUM(Q29:Q30)*30+R29</f>
         <v>878</v>
       </c>
-      <c r="R31" s="45"/>
+      <c r="R31" s="49"/>
       <c r="U31" s="33"/>
       <c r="W31" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X31" s="44">
+        <v>10</v>
+      </c>
+      <c r="X31" s="48">
         <f>SUM(X30:X30)*30+Y30</f>
         <v>120</v>
       </c>
-      <c r="Y31" s="45"/>
+      <c r="Y31" s="49"/>
       <c r="AB31" s="7"/>
     </row>
     <row r="32" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C32" s="44">
-        <f>SUM(C30:C31)*24+D30</f>
-        <v>3192</v>
-      </c>
-      <c r="D32" s="45"/>
-      <c r="F32" s="7"/>
+      <c r="B32" s="45">
+        <v>158234</v>
+      </c>
+      <c r="C32" s="7">
+        <v>74</v>
+      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="8">
+        <v>46191</v>
+      </c>
+      <c r="F32" s="9">
+        <f>(E32-$AC$1)/365*12</f>
+        <v>18.871232876712327</v>
+      </c>
       <c r="G32" s="33"/>
-      <c r="H32" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="I32" s="7">
-        <v>156609</v>
-      </c>
-      <c r="J32" s="7">
-        <v>2</v>
-      </c>
-      <c r="K32" s="7">
-        <v>23</v>
-      </c>
-      <c r="L32" s="8">
-        <v>46183</v>
-      </c>
-      <c r="M32" s="9">
-        <f t="shared" ref="M32:M34" si="35">(L32-$AC$1)/365*12</f>
-        <v>18.608219178082194</v>
-      </c>
+      <c r="I32" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J32" s="48">
+        <f>SUM(J31)*30+K31</f>
+        <v>242</v>
+      </c>
+      <c r="K32" s="49"/>
       <c r="N32" s="33"/>
       <c r="U32" s="33"/>
       <c r="AB32" s="7"/>
     </row>
-    <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="48"/>
+    <row r="33" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="C33" s="7">
+        <v>111</v>
+      </c>
       <c r="D33" s="7"/>
-      <c r="F33" s="7"/>
+      <c r="E33" s="8">
+        <v>46211</v>
+      </c>
+      <c r="F33" s="9">
+        <f>(E33-$AC$1)/365*12</f>
+        <v>19.528767123287672</v>
+      </c>
       <c r="G33" s="33"/>
-      <c r="I33" s="7">
-        <v>156609</v>
-      </c>
-      <c r="J33" s="7">
-        <v>6</v>
-      </c>
       <c r="K33" s="7"/>
-      <c r="L33" s="8">
-        <v>46183</v>
-      </c>
-      <c r="M33" s="9">
-        <f t="shared" ref="M33" si="36">(L33-$AC$1)/365*12</f>
-        <v>18.608219178082194</v>
-      </c>
       <c r="N33" s="33"/>
       <c r="O33" s="6" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="P33" s="7" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="Q33" s="7">
         <v>10</v>
@@ -2765,7 +2799,7 @@
       </c>
       <c r="U33" s="33"/>
       <c r="V33" s="6" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="W33" s="11"/>
       <c r="X33" s="7"/>
@@ -2775,44 +2809,39 @@
       <c r="AB33" s="7"/>
     </row>
     <row r="34" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B34" s="49">
-        <v>158233</v>
-      </c>
-      <c r="C34" s="7">
-        <v>0</v>
-      </c>
-      <c r="D34" s="7">
-        <v>22</v>
-      </c>
-      <c r="E34" s="8">
-        <v>46249</v>
-      </c>
-      <c r="F34" s="9">
-        <f>(E34-$AC$1)/365*12</f>
-        <v>20.778082191780822</v>
-      </c>
+      <c r="B34" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="48">
+        <f>SUM(C30:C33)*24+D30</f>
+        <v>5868</v>
+      </c>
+      <c r="D34" s="49"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="33"/>
+      <c r="H34" s="17" t="s">
+        <v>86</v>
+      </c>
       <c r="I34" s="7">
-        <v>162839</v>
-      </c>
-      <c r="J34" s="11">
-        <v>77</v>
-      </c>
-      <c r="K34" s="7"/>
+        <v>156609</v>
+      </c>
+      <c r="J34" s="7">
+        <v>2</v>
+      </c>
+      <c r="K34" s="7">
+        <v>23</v>
+      </c>
       <c r="L34" s="8">
-        <v>46305</v>
+        <v>46183</v>
       </c>
       <c r="M34" s="9">
-        <f t="shared" si="35"/>
-        <v>22.61917808219178</v>
+        <f t="shared" ref="M34:M36" si="36">(L34-$AC$1)/365*12</f>
+        <v>18.608219178082194</v>
       </c>
       <c r="N34" s="33"/>
       <c r="O34" s="6"/>
       <c r="P34" s="7" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="Q34" s="7">
         <v>26</v>
@@ -2828,7 +2857,7 @@
       <c r="U34" s="33"/>
       <c r="V34" s="11"/>
       <c r="W34" s="11" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="X34" s="11">
         <v>0</v>
@@ -2846,64 +2875,81 @@
       <c r="AB34" s="7"/>
     </row>
     <row r="35" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="27"/>
-      <c r="B35" s="49">
-        <v>158233</v>
-      </c>
-      <c r="C35" s="7">
-        <v>157</v>
-      </c>
+      <c r="B35" s="44"/>
       <c r="D35" s="7"/>
-      <c r="E35" s="8">
-        <v>46249</v>
-      </c>
-      <c r="F35" s="9">
-        <f>(E35-$AC$1)/365*12</f>
-        <v>20.778082191780822</v>
-      </c>
+      <c r="F35" s="7"/>
       <c r="G35" s="33"/>
-      <c r="I35" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J35" s="44">
-        <f>SUM(J32:J34)*24+K32</f>
-        <v>2063</v>
-      </c>
-      <c r="K35" s="45"/>
+      <c r="I35" s="7">
+        <v>156609</v>
+      </c>
+      <c r="J35" s="7">
+        <v>6</v>
+      </c>
+      <c r="K35" s="7"/>
+      <c r="L35" s="8">
+        <v>46183</v>
+      </c>
+      <c r="M35" s="9">
+        <f t="shared" ref="M35" si="38">(L35-$AC$1)/365*12</f>
+        <v>18.608219178082194</v>
+      </c>
       <c r="N35" s="33"/>
       <c r="P35" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q35" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q35" s="48">
         <f>SUM(Q33:Q34)*30+R33</f>
         <v>1098</v>
       </c>
-      <c r="R35" s="45"/>
+      <c r="R35" s="49"/>
       <c r="S35" s="7"/>
       <c r="T35" s="7"/>
       <c r="U35" s="33"/>
       <c r="W35" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X35" s="44">
+        <v>10</v>
+      </c>
+      <c r="X35" s="48">
         <f>SUM(X33:X34)*18+Y33</f>
         <v>0</v>
       </c>
-      <c r="Y35" s="45"/>
+      <c r="Y35" s="49"/>
       <c r="AB35" s="7"/>
     </row>
     <row r="36" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B36" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C36" s="44">
-        <f>SUM(C34)*24+D34</f>
+      <c r="A36" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="45">
+        <v>158233</v>
+      </c>
+      <c r="C36" s="7">
+        <v>0</v>
+      </c>
+      <c r="D36" s="7">
         <v>22</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="F36" s="7"/>
+      <c r="E36" s="8">
+        <v>46249</v>
+      </c>
+      <c r="F36" s="9">
+        <f>(E36-$AC$1)/365*12</f>
+        <v>20.778082191780822</v>
+      </c>
       <c r="G36" s="33"/>
+      <c r="I36" s="7">
+        <v>162839</v>
+      </c>
+      <c r="J36" s="11">
+        <v>77</v>
+      </c>
       <c r="K36" s="7"/>
+      <c r="L36" s="8">
+        <v>46305</v>
+      </c>
+      <c r="M36" s="9">
+        <f t="shared" si="36"/>
+        <v>22.61917808219178</v>
+      </c>
       <c r="N36" s="33"/>
       <c r="P36" s="13"/>
       <c r="R36" s="30"/>
@@ -2912,36 +2958,37 @@
       <c r="U36" s="33"/>
       <c r="AB36" s="7"/>
     </row>
-    <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="48"/>
+    <row r="37" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="27"/>
+      <c r="B37" s="45">
+        <v>158233</v>
+      </c>
+      <c r="C37" s="7">
+        <v>44</v>
+      </c>
       <c r="D37" s="7"/>
-      <c r="F37" s="7"/>
+      <c r="E37" s="8">
+        <v>46249</v>
+      </c>
+      <c r="F37" s="9">
+        <f>(E37-$AC$1)/365*12</f>
+        <v>20.778082191780822</v>
+      </c>
       <c r="G37" s="33"/>
-      <c r="H37" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="I37" s="7">
-        <v>158210</v>
-      </c>
-      <c r="J37" s="7">
-        <v>0</v>
-      </c>
-      <c r="K37" s="7">
+      <c r="I37" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L37" s="8">
-        <v>46282</v>
-      </c>
-      <c r="M37" s="9">
-        <f t="shared" ref="M37:M38" si="38">(L37-$AC$1)/365*12</f>
-        <v>21.863013698630137</v>
-      </c>
+      <c r="J37" s="48">
+        <f>SUM(J34:J36)*24+K34</f>
+        <v>2063</v>
+      </c>
+      <c r="K37" s="49"/>
       <c r="N37" s="33"/>
       <c r="O37" s="6" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="P37" s="7" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="Q37" s="7">
         <v>4</v>
@@ -2958,10 +3005,10 @@
       </c>
       <c r="U37" s="33"/>
       <c r="V37" s="6" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="W37" s="7" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="X37" s="7">
         <v>1</v>
@@ -2979,44 +3026,27 @@
       <c r="AB37" s="7"/>
     </row>
     <row r="38" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="6" t="s">
+      <c r="A38" s="27"/>
+      <c r="B38" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B38" s="49" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="11">
-        <v>16</v>
-      </c>
-      <c r="D38" s="7">
-        <v>0</v>
-      </c>
-      <c r="E38" s="14">
-        <v>46260</v>
+      <c r="C38" s="7">
+        <v>107</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="8">
+        <v>46282</v>
       </c>
       <c r="F38" s="9">
         <f>(E38-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
+        <v>21.863013698630137</v>
       </c>
       <c r="G38" s="33"/>
-      <c r="I38" s="7">
-        <v>161789</v>
-      </c>
-      <c r="J38" s="7">
-        <v>91</v>
-      </c>
       <c r="K38" s="7"/>
-      <c r="L38" s="8">
-        <v>46305</v>
-      </c>
-      <c r="M38" s="9">
-        <f t="shared" si="38"/>
-        <v>22.61917808219178</v>
-      </c>
       <c r="N38" s="33"/>
       <c r="O38" s="24"/>
       <c r="P38" s="7" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="Q38" s="7">
         <v>46</v>
@@ -3037,96 +3067,110 @@
       <c r="AB38" s="7"/>
     </row>
     <row r="39" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="49" t="s">
-        <v>83</v>
-      </c>
-      <c r="C39" s="41">
-        <v>79</v>
-      </c>
-      <c r="D39" s="7">
-        <v>34</v>
-      </c>
-      <c r="E39" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F39" s="9">
-        <f>(E39-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
-      </c>
+      <c r="B39" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" s="48">
+        <f>SUM(C36:C38)*24+D36</f>
+        <v>3646</v>
+      </c>
+      <c r="D39" s="49"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="33"/>
-      <c r="I39" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J39" s="44">
-        <f>SUM(J37:J38)*24+K37</f>
-        <v>2194</v>
-      </c>
-      <c r="K39" s="45"/>
+      <c r="H39" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="I39" s="7">
+        <v>158210</v>
+      </c>
+      <c r="J39" s="7">
+        <v>0</v>
+      </c>
+      <c r="K39" s="7">
+        <v>10</v>
+      </c>
+      <c r="L39" s="8">
+        <v>46282</v>
+      </c>
+      <c r="M39" s="9">
+        <f t="shared" ref="M39:M40" si="40">(L39-$AC$1)/365*12</f>
+        <v>21.863013698630137</v>
+      </c>
       <c r="N39" s="33"/>
       <c r="P39" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q39" s="44">
+        <v>10</v>
+      </c>
+      <c r="Q39" s="48">
         <f>SUM(Q37:Q38)*30+R37</f>
         <v>1520</v>
       </c>
-      <c r="R39" s="45"/>
+      <c r="R39" s="49"/>
       <c r="U39" s="33"/>
       <c r="W39" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="X39" s="44">
+        <v>10</v>
+      </c>
+      <c r="X39" s="48">
         <f>SUM(X37:X38)*18+Y37</f>
         <v>24</v>
       </c>
-      <c r="Y39" s="45"/>
+      <c r="Y39" s="49"/>
       <c r="AB39" s="7"/>
     </row>
     <row r="40" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B40" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C40" s="44">
-        <f>SUM(C38:C39)*30+D38+D39</f>
-        <v>2884</v>
-      </c>
-      <c r="D40" s="45"/>
+      <c r="B40" s="44"/>
+      <c r="D40" s="7"/>
       <c r="F40" s="7"/>
       <c r="G40" s="33"/>
-      <c r="I40" s="13"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
+      <c r="I40" s="7">
+        <v>161789</v>
+      </c>
+      <c r="J40" s="7">
+        <v>91</v>
+      </c>
+      <c r="K40" s="7"/>
+      <c r="L40" s="8">
+        <v>46305</v>
+      </c>
+      <c r="M40" s="9">
+        <f t="shared" si="40"/>
+        <v>22.61917808219178</v>
+      </c>
       <c r="N40" s="33"/>
       <c r="U40" s="34"/>
       <c r="AB40" s="7"/>
     </row>
     <row r="41" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B41" s="48"/>
-      <c r="D41" s="7"/>
-      <c r="F41" s="7"/>
+      <c r="A41" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="11">
+        <v>16</v>
+      </c>
+      <c r="D41" s="7">
+        <v>0</v>
+      </c>
+      <c r="E41" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F41" s="9">
+        <f>(E41-$AC$1)/365*12</f>
+        <v>21.139726027397259</v>
+      </c>
       <c r="G41" s="33"/>
-      <c r="H41" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I41" s="7">
-        <v>156642</v>
-      </c>
-      <c r="J41" s="11">
-        <v>4</v>
-      </c>
-      <c r="K41" s="7">
-        <v>19</v>
-      </c>
-      <c r="L41" s="8">
-        <v>46197</v>
-      </c>
-      <c r="M41" s="9">
-        <f t="shared" ref="M41:M42" si="40">(L41-$AC$1)/365*12</f>
-        <v>19.06849315068493</v>
-      </c>
+      <c r="I41" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J41" s="48">
+        <f>SUM(J39:J40)*24+K39</f>
+        <v>2194</v>
+      </c>
+      <c r="K41" s="49"/>
       <c r="N41" s="33"/>
       <c r="O41" s="6" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="P41" s="7">
         <v>17</v>
@@ -3135,74 +3179,64 @@
       <c r="AB41" s="7"/>
     </row>
     <row r="42" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B42" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="C42" s="7">
-        <v>9</v>
+      <c r="B42" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="C42" s="41">
+        <v>79</v>
       </c>
       <c r="D42" s="7">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E42" s="14">
-        <v>46260</v>
+        <v>46291</v>
       </c>
       <c r="F42" s="9">
         <f>(E42-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
+        <v>22.158904109589042</v>
       </c>
       <c r="G42" s="33"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="7">
-        <v>156642</v>
-      </c>
-      <c r="J42" s="11">
-        <v>51</v>
-      </c>
-      <c r="K42" s="7"/>
-      <c r="L42" s="8">
-        <v>46197</v>
-      </c>
-      <c r="M42" s="9">
-        <f t="shared" si="40"/>
-        <v>19.06849315068493</v>
-      </c>
+      <c r="I42" s="13"/>
+      <c r="J42" s="30"/>
+      <c r="K42" s="30"/>
       <c r="N42" s="33"/>
       <c r="P42" s="7"/>
       <c r="U42" s="24"/>
       <c r="AB42" s="7"/>
     </row>
     <row r="43" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="6"/>
-      <c r="B43" s="49" t="s">
-        <v>76</v>
-      </c>
-      <c r="C43" s="7">
-        <v>13</v>
-      </c>
-      <c r="D43" s="7"/>
-      <c r="E43" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F43" s="9">
-        <f>(E43-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
-      </c>
+      <c r="B43" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" s="48">
+        <f>SUM(C41:C42)*30+D41+D42</f>
+        <v>2884</v>
+      </c>
+      <c r="D43" s="49"/>
+      <c r="F43" s="7"/>
       <c r="G43" s="33"/>
-      <c r="I43" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J43" s="44">
-        <f>SUM(J41:J42)*24+K41</f>
-        <v>1339</v>
-      </c>
-      <c r="K43" s="45"/>
+      <c r="H43" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="I43" s="7">
+        <v>156642</v>
+      </c>
+      <c r="J43" s="11">
+        <v>4</v>
+      </c>
+      <c r="K43" s="7">
+        <v>19</v>
+      </c>
+      <c r="L43" s="8">
+        <v>46197</v>
+      </c>
+      <c r="M43" s="9">
+        <f t="shared" ref="M43:M44" si="41">(L43-$AC$1)/365*12</f>
+        <v>19.06849315068493</v>
+      </c>
       <c r="N43" s="33"/>
       <c r="O43" s="6" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="P43" s="7">
         <v>52</v>
@@ -3211,273 +3245,290 @@
       <c r="AB43" s="7"/>
     </row>
     <row r="44" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
-      <c r="B44" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="C44" s="7">
-        <v>68</v>
-      </c>
+      <c r="B44" s="44"/>
       <c r="D44" s="7"/>
-      <c r="E44" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F44" s="9">
-        <f>(E44-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
-      </c>
+      <c r="F44" s="7"/>
       <c r="G44" s="33"/>
+      <c r="H44" s="27"/>
+      <c r="I44" s="7">
+        <v>156642</v>
+      </c>
+      <c r="J44" s="11">
+        <v>51</v>
+      </c>
       <c r="K44" s="7"/>
+      <c r="L44" s="8">
+        <v>46197</v>
+      </c>
+      <c r="M44" s="9">
+        <f t="shared" si="41"/>
+        <v>19.06849315068493</v>
+      </c>
       <c r="N44" s="33"/>
       <c r="U44" s="24"/>
       <c r="AB44" s="7"/>
     </row>
     <row r="45" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B45" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C45" s="44">
-        <f>SUM(C43:C44)*30+D43+D44</f>
-        <v>2430</v>
-      </c>
-      <c r="D45" s="45"/>
-      <c r="F45" s="7"/>
+      <c r="A45" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B45" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C45" s="7">
+        <v>9</v>
+      </c>
+      <c r="D45" s="7">
+        <v>0</v>
+      </c>
+      <c r="E45" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F45" s="9">
+        <f>(E45-$AC$1)/365*12</f>
+        <v>21.139726027397259</v>
+      </c>
       <c r="G45" s="33"/>
-      <c r="H45" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="I45" s="7">
-        <v>156641</v>
-      </c>
-      <c r="J45" s="7">
-        <v>2</v>
-      </c>
-      <c r="K45" s="7">
-        <v>23</v>
-      </c>
-      <c r="L45" s="8">
-        <v>46197</v>
-      </c>
-      <c r="M45" s="9">
-        <f t="shared" ref="M45:M47" si="41">(L45-$AC$1)/365*12</f>
-        <v>19.06849315068493</v>
-      </c>
+      <c r="I45" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J45" s="48">
+        <f>SUM(J43:J44)*24+K43</f>
+        <v>1339</v>
+      </c>
+      <c r="K45" s="49"/>
       <c r="N45" s="33"/>
       <c r="S45" s="4"/>
       <c r="U45" s="24"/>
       <c r="AB45" s="7"/>
     </row>
     <row r="46" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="48"/>
+      <c r="A46" s="6"/>
+      <c r="B46" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="C46" s="7">
+        <v>13</v>
+      </c>
       <c r="D46" s="7"/>
-      <c r="F46" s="7"/>
+      <c r="E46" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F46" s="9">
+        <f>(E46-$AC$1)/365*12</f>
+        <v>21.139726027397259</v>
+      </c>
       <c r="G46" s="33"/>
-      <c r="I46" s="7">
-        <v>156641</v>
-      </c>
-      <c r="J46" s="7">
-        <v>21</v>
-      </c>
       <c r="K46" s="7"/>
-      <c r="L46" s="8">
-        <v>46197</v>
-      </c>
-      <c r="M46" s="9">
-        <f t="shared" ref="M46" si="42">(L46-$AC$1)/365*12</f>
-        <v>19.06849315068493</v>
-      </c>
       <c r="N46" s="33"/>
       <c r="U46" s="24"/>
       <c r="AB46" s="7"/>
     </row>
     <row r="47" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A47" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B47" s="49" t="s">
-        <v>78</v>
+      <c r="A47" s="6"/>
+      <c r="B47" s="45" t="s">
+        <v>60</v>
       </c>
       <c r="C47" s="7">
-        <v>3</v>
-      </c>
-      <c r="D47" s="15">
+        <v>68</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="14">
+        <v>46291</v>
+      </c>
+      <c r="F47" s="9">
+        <f>(E47-$AC$1)/365*12</f>
+        <v>22.158904109589042</v>
+      </c>
+      <c r="G47" s="33"/>
+      <c r="H47" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="I47" s="7">
+        <v>156641</v>
+      </c>
+      <c r="J47" s="7">
+        <v>2</v>
+      </c>
+      <c r="K47" s="7">
         <v>23</v>
       </c>
-      <c r="E47" s="14">
-        <v>46199</v>
-      </c>
-      <c r="F47" s="9">
-        <f t="shared" ref="F47" si="43">(E47-$AC$1)/365*12</f>
-        <v>19.134246575342466</v>
-      </c>
-      <c r="G47" s="33"/>
-      <c r="I47" s="7">
-        <v>162040</v>
-      </c>
-      <c r="J47" s="7">
-        <v>84</v>
-      </c>
-      <c r="K47" s="7"/>
       <c r="L47" s="8">
-        <v>46303</v>
+        <v>46197</v>
       </c>
       <c r="M47" s="9">
-        <f t="shared" si="41"/>
-        <v>22.553424657534247</v>
+        <f t="shared" ref="M47:M49" si="42">(L47-$AC$1)/365*12</f>
+        <v>19.06849315068493</v>
       </c>
       <c r="N47" s="33"/>
       <c r="U47" s="24"/>
       <c r="AB47" s="7"/>
     </row>
     <row r="48" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="6"/>
-      <c r="B48" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="C48" s="11">
-        <v>54</v>
-      </c>
-      <c r="D48" s="15">
-        <v>7</v>
-      </c>
-      <c r="E48" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F48" s="9">
-        <f t="shared" ref="F48" si="44">(E48-$AC$1)/365*12</f>
-        <v>22.158904109589042</v>
-      </c>
+      <c r="B48" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="48">
+        <f>SUM(C46:C47)*30+D46+D47</f>
+        <v>2430</v>
+      </c>
+      <c r="D48" s="49"/>
+      <c r="F48" s="7"/>
       <c r="G48" s="33"/>
-      <c r="H48" s="36"/>
-      <c r="I48" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="J48" s="44">
-        <f>SUM(J45:J47)*24+K45</f>
-        <v>2591</v>
-      </c>
-      <c r="K48" s="45"/>
+      <c r="I48" s="7">
+        <v>156641</v>
+      </c>
+      <c r="J48" s="7">
+        <v>21</v>
+      </c>
+      <c r="K48" s="7"/>
+      <c r="L48" s="8">
+        <v>46197</v>
+      </c>
+      <c r="M48" s="9">
+        <f t="shared" ref="M48" si="43">(L48-$AC$1)/365*12</f>
+        <v>19.06849315068493</v>
+      </c>
       <c r="N48" s="33"/>
       <c r="U48" s="24"/>
       <c r="AB48" s="7"/>
     </row>
     <row r="49" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B49" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C49" s="44">
-        <f>SUM(C47:C48)*30+D47+D48</f>
-        <v>1740</v>
-      </c>
-      <c r="D49" s="45"/>
+      <c r="B49" s="44"/>
+      <c r="D49" s="7"/>
       <c r="F49" s="7"/>
       <c r="G49" s="33"/>
-      <c r="H49" s="24"/>
+      <c r="I49" s="7">
+        <v>162040</v>
+      </c>
+      <c r="J49" s="7">
+        <v>84</v>
+      </c>
       <c r="K49" s="7"/>
+      <c r="L49" s="8">
+        <v>46303</v>
+      </c>
+      <c r="M49" s="9">
+        <f t="shared" si="42"/>
+        <v>22.553424657534247</v>
+      </c>
       <c r="N49" s="33"/>
       <c r="U49" s="24"/>
       <c r="AB49" s="7"/>
     </row>
-    <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B50" s="48"/>
-      <c r="D50" s="7"/>
-      <c r="F50" s="7"/>
+    <row r="50" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B50" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="C50" s="7">
+        <v>3</v>
+      </c>
+      <c r="D50" s="15">
+        <v>23</v>
+      </c>
+      <c r="E50" s="14">
+        <v>46199</v>
+      </c>
+      <c r="F50" s="9">
+        <f t="shared" ref="F50" si="44">(E50-$AC$1)/365*12</f>
+        <v>19.134246575342466</v>
+      </c>
       <c r="G50" s="40"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-      <c r="L50" s="37"/>
-      <c r="M50" s="38"/>
+      <c r="H50" s="36"/>
+      <c r="I50" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J50" s="48">
+        <f>SUM(J47:J49)*24+K47</f>
+        <v>2591</v>
+      </c>
+      <c r="K50" s="49"/>
       <c r="N50" s="24"/>
       <c r="U50" s="24"/>
       <c r="AB50" s="7"/>
     </row>
-    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="B51" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51" s="7">
-        <v>17</v>
-      </c>
-      <c r="D51" s="11">
-        <v>31</v>
+    <row r="51" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="6"/>
+      <c r="B51" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C51" s="11">
+        <v>54</v>
+      </c>
+      <c r="D51" s="15">
+        <v>7</v>
       </c>
       <c r="E51" s="14">
-        <v>46260</v>
+        <v>46291</v>
       </c>
       <c r="F51" s="9">
-        <f t="shared" ref="F51:F53" si="45">(E51-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
+        <f t="shared" ref="F51" si="45">(E51-$AC$1)/365*12</f>
+        <v>22.158904109589042</v>
       </c>
       <c r="G51" s="33"/>
-      <c r="I51" s="39"/>
-      <c r="J51" s="47"/>
-      <c r="K51" s="47"/>
-      <c r="L51" s="24"/>
-      <c r="M51" s="24"/>
+      <c r="H51" s="24"/>
+      <c r="K51" s="7"/>
       <c r="N51" s="24"/>
       <c r="U51" s="24"/>
       <c r="AB51" s="7"/>
     </row>
-    <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="6"/>
-      <c r="B52" s="48" t="s">
-        <v>80</v>
-      </c>
-      <c r="C52" s="7">
-        <v>5</v>
-      </c>
-      <c r="D52" s="11">
-        <v>7</v>
-      </c>
-      <c r="E52" s="14">
-        <v>46260</v>
-      </c>
-      <c r="F52" s="9">
-        <f t="shared" ref="F52" si="46">(E52-$AC$1)/365*12</f>
-        <v>21.139726027397259</v>
-      </c>
+    <row r="52" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52" s="48">
+        <f>SUM(C50:C51)*30+D50+D51</f>
+        <v>1740</v>
+      </c>
+      <c r="D52" s="49"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="33"/>
-      <c r="K52" s="7"/>
+      <c r="I52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="37"/>
+      <c r="M52" s="38"/>
       <c r="N52" s="24"/>
       <c r="U52" s="24"/>
       <c r="AB52" s="7"/>
     </row>
-    <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="6"/>
-      <c r="B53" s="48" t="s">
-        <v>86</v>
-      </c>
-      <c r="C53" s="7">
-        <v>31</v>
-      </c>
-      <c r="D53" s="11"/>
-      <c r="E53" s="14">
-        <v>46291</v>
-      </c>
-      <c r="F53" s="9">
-        <f t="shared" si="45"/>
-        <v>22.158904109589042</v>
-      </c>
+    <row r="53" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B53" s="44"/>
+      <c r="D53" s="7"/>
+      <c r="F53" s="7"/>
       <c r="G53" s="33"/>
-      <c r="K53" s="7"/>
+      <c r="I53" s="39"/>
+      <c r="J53" s="51"/>
+      <c r="K53" s="51"/>
+      <c r="L53" s="24"/>
+      <c r="M53" s="24"/>
       <c r="N53" s="24"/>
       <c r="U53" s="24"/>
       <c r="AB53" s="7"/>
     </row>
-    <row r="54" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B54" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C54" s="44" cm="1">
-        <f t="array" ref="C54">SUM(C51:C53*40)+D51+D53</f>
-        <v>2151</v>
-      </c>
-      <c r="D54" s="45"/>
-      <c r="F54" s="7"/>
+    <row r="54" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="B54" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C54" s="7">
+        <v>17</v>
+      </c>
+      <c r="D54" s="11">
+        <v>31</v>
+      </c>
+      <c r="E54" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F54" s="9">
+        <f t="shared" ref="F54:F56" si="46">(E54-$AC$1)/365*12</f>
+        <v>21.139726027397259</v>
+      </c>
       <c r="G54" s="33"/>
       <c r="K54" s="7"/>
       <c r="N54" s="24"/>
@@ -3485,33 +3536,43 @@
       <c r="AB54" s="7"/>
     </row>
     <row r="55" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B55" s="48"/>
-      <c r="D55" s="7"/>
-      <c r="F55" s="7"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="C55" s="7">
+        <v>5</v>
+      </c>
+      <c r="D55" s="11">
+        <v>7</v>
+      </c>
+      <c r="E55" s="14">
+        <v>46260</v>
+      </c>
+      <c r="F55" s="9">
+        <f t="shared" ref="F55" si="47">(E55-$AC$1)/365*12</f>
+        <v>21.139726027397259</v>
+      </c>
       <c r="G55" s="33"/>
       <c r="K55" s="7"/>
       <c r="U55" s="24"/>
       <c r="AB55" s="7"/>
     </row>
     <row r="56" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B56" s="49" t="s">
-        <v>82</v>
+      <c r="A56" s="6"/>
+      <c r="B56" s="44" t="s">
+        <v>62</v>
       </c>
       <c r="C56" s="7">
-        <v>10</v>
-      </c>
-      <c r="D56" s="7">
-        <v>19</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D56" s="11"/>
       <c r="E56" s="14">
-        <v>45528</v>
-      </c>
-      <c r="F56" s="16">
-        <f>(E56-$AC$1)/365*12</f>
-        <v>-2.9260273972602739</v>
+        <v>46291</v>
+      </c>
+      <c r="F56" s="9">
+        <f t="shared" si="46"/>
+        <v>22.158904109589042</v>
       </c>
       <c r="G56" s="33"/>
       <c r="K56" s="7"/>
@@ -3519,14 +3580,14 @@
       <c r="AB56" s="7"/>
     </row>
     <row r="57" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B57" s="50" t="s">
-        <v>13</v>
-      </c>
-      <c r="C57" s="44">
-        <f>SUM(C56)*30+D56</f>
-        <v>319</v>
-      </c>
-      <c r="D57" s="45"/>
+      <c r="B57" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C57" s="48" cm="1">
+        <f t="array" ref="C57">SUM(C54:C56*40)+D54+D56</f>
+        <v>2151</v>
+      </c>
+      <c r="D57" s="49"/>
       <c r="F57" s="7"/>
       <c r="G57" s="33"/>
       <c r="K57" s="7"/>
@@ -3534,6 +3595,7 @@
       <c r="AB57" s="7"/>
     </row>
     <row r="58" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B58" s="44"/>
       <c r="D58" s="7"/>
       <c r="F58" s="7"/>
       <c r="G58" s="34"/>
@@ -3541,15 +3603,39 @@
       <c r="U58" s="24"/>
       <c r="AB58" s="7"/>
     </row>
-    <row r="59" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D59" s="7"/>
-      <c r="F59" s="7"/>
+    <row r="59" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="C59" s="7">
+        <v>10</v>
+      </c>
+      <c r="D59" s="7">
+        <v>19</v>
+      </c>
+      <c r="E59" s="14">
+        <v>45528</v>
+      </c>
+      <c r="F59" s="16">
+        <f>(E59-$AC$1)/365*12</f>
+        <v>-2.9260273972602739</v>
+      </c>
       <c r="G59" s="40"/>
       <c r="K59" s="7"/>
       <c r="AB59" s="7"/>
     </row>
-    <row r="60" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D60" s="7"/>
+    <row r="60" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B60" s="46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C60" s="48">
+        <f>SUM(C59)*30+D59</f>
+        <v>319</v>
+      </c>
+      <c r="D60" s="49"/>
       <c r="F60" s="7"/>
       <c r="G60" s="33"/>
       <c r="K60" s="7"/>
@@ -4327,7 +4413,6 @@
     <row r="186" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D186" s="7"/>
       <c r="F186" s="7"/>
-      <c r="H186"/>
       <c r="K186" s="7"/>
       <c r="O186"/>
       <c r="P186"/>
@@ -4340,7 +4425,6 @@
     <row r="187" spans="1:28" s="10" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D187" s="7"/>
       <c r="F187" s="7"/>
-      <c r="H187"/>
       <c r="K187" s="7"/>
       <c r="O187"/>
       <c r="P187"/>
@@ -4354,11 +4438,7 @@
       <c r="D188" s="7"/>
       <c r="F188" s="7"/>
       <c r="H188"/>
-      <c r="I188"/>
-      <c r="J188"/>
-      <c r="K188" s="4"/>
-      <c r="L188"/>
-      <c r="M188"/>
+      <c r="K188" s="7"/>
       <c r="O188"/>
       <c r="P188"/>
       <c r="Q188"/>
@@ -4371,11 +4451,7 @@
       <c r="D189" s="7"/>
       <c r="F189" s="7"/>
       <c r="H189"/>
-      <c r="I189"/>
-      <c r="J189"/>
-      <c r="K189" s="4"/>
-      <c r="L189"/>
-      <c r="M189"/>
+      <c r="K189" s="7"/>
       <c r="O189"/>
       <c r="P189"/>
       <c r="Q189"/>
@@ -4467,9 +4543,30 @@
       <c r="E196" s="10"/>
       <c r="F196" s="7"/>
     </row>
-    <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A197" s="10"/>
+      <c r="B197" s="10"/>
+      <c r="C197" s="10"/>
+      <c r="D197" s="7"/>
+      <c r="E197" s="10"/>
+      <c r="F197" s="7"/>
+    </row>
+    <row r="198" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A198" s="10"/>
+      <c r="B198" s="10"/>
+      <c r="C198" s="10"/>
+      <c r="D198" s="7"/>
+      <c r="E198" s="10"/>
+      <c r="F198" s="7"/>
+    </row>
+    <row r="199" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A199" s="10"/>
+      <c r="B199" s="10"/>
+      <c r="C199" s="10"/>
+      <c r="D199" s="7"/>
+      <c r="E199" s="10"/>
+      <c r="F199" s="7"/>
+    </row>
     <row r="200" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="201" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="202" spans="1:6" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4555,39 +4652,39 @@
     <row r="282" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="283" ht="27.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="dQ/EmLJdRy+LEjUdegNTd6elxTW6x4wPJMcqKzoJ23HGROJUDroRl269gsk8ntNGYgtDbi0wfubNe8kxfexKuQ==" saltValue="+1lPGLnb7c7QYkETes/9RQ==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
+  <sheetProtection formatCells="0" formatColumns="0" formatRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C52:D52"/>
+    <mergeCell ref="C60:D60"/>
     <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="J23:K23"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="J48:K48"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="J50:K50"/>
     <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
     <mergeCell ref="J6:K6"/>
     <mergeCell ref="J10:K10"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="J19:K19"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="J21:K21"/>
     <mergeCell ref="X39:Y39"/>
-    <mergeCell ref="J51:K51"/>
+    <mergeCell ref="J53:K53"/>
     <mergeCell ref="Q6:R6"/>
     <mergeCell ref="Q10:R10"/>
     <mergeCell ref="Q14:R14"/>
     <mergeCell ref="Q22:R22"/>
     <mergeCell ref="Q27:R27"/>
     <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="J27:K27"/>
-    <mergeCell ref="J30:K30"/>
-    <mergeCell ref="J35:K35"/>
-    <mergeCell ref="J39:K39"/>
-    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="J29:K29"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="J37:K37"/>
+    <mergeCell ref="J41:K41"/>
+    <mergeCell ref="J45:K45"/>
     <mergeCell ref="X35:Y35"/>
     <mergeCell ref="Q18:R18"/>
     <mergeCell ref="Q35:R35"/>

</xml_diff>